<commit_message>
Teste de SquadLanes, não funcionando
</commit_message>
<xml_diff>
--- a/database/dados.xlsx
+++ b/database/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Desenvolvimento\Web\squad-admin-js\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5C3919-3551-443F-8D5D-6B4374D20286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AC9845-CE8E-4A38-AE39-67ECF4F21E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="15585" windowHeight="11385" tabRatio="743" activeTab="5" xr2:uid="{D957AD89-D5EE-4E04-827D-F6CC1DBEEFE0}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="15585" windowHeight="11385" tabRatio="743" activeTab="4" xr2:uid="{D957AD89-D5EE-4E04-827D-F6CC1DBEEFE0}"/>
   </bookViews>
   <sheets>
     <sheet name="mapas" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2805" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2804" uniqueCount="577">
   <si>
     <t>1. REGRAS DE COMPORTAMENTO</t>
   </si>
@@ -1730,9 +1730,6 @@
   </si>
   <si>
     <t>Regra 3.1 - Monotripulando veículo</t>
-  </si>
-  <si>
-    <t>Prezados jogadores, está sendo realizado uma pesquisa sobre as regras de sitiar main base inimiga. Acesse nosso Discord no canal avisos. Serão sorteados 2 VIP's aos participantes! Obrigado a todos e bom jogo!</t>
   </si>
   <si>
     <t>time_day</t>
@@ -2334,7 +2331,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -2467,7 +2464,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -2547,43 +2544,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
+        <v>559</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>560</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="22" t="s">
+        <v>557</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>558</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>561</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>558</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>559</v>
-      </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>562</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>563</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>564</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="I1" s="17" t="s">
         <v>565</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>566</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>567</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="L1" s="22" t="s">
         <v>568</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>569</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -14750,7 +14747,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -15033,8 +15030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE61EF27-4215-440C-A8D0-D56239102DC7}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -15045,7 +15042,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -15088,10 +15085,8 @@
         <v>424</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>557</v>
-      </c>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -15103,7 +15098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38936B9-5690-42EA-87FB-9BF3E91F3C5E}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -15115,12 +15110,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
@@ -15209,10 +15204,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>570</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>571</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>